<commit_message>
Test to fetch db details from Excel file
</commit_message>
<xml_diff>
--- a/TestData/Database.xlsx
+++ b/TestData/Database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JW233CE\BPxPoc\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10656162\MyProject\BPxPoc\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78CF5F82-263B-44E9-BAE4-BA0829A4B29A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5FF94EF-9AB2-4C15-8692-FFD662F0160C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2670" yWindow="2745" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,30 +25,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>${DB_Server_Name}</t>
-  </si>
-  <si>
-    <t>Test name</t>
-  </si>
-  <si>
-    <t>${DBUser_Name}</t>
-  </si>
-  <si>
-    <t>Test user name</t>
-  </si>
-  <si>
-    <t>${DB_password}</t>
-  </si>
-  <si>
-    <t>${DB_name}</t>
-  </si>
-  <si>
-    <t>Test password</t>
-  </si>
-  <si>
-    <t>Test db name</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>${DB_Name}</t>
+  </si>
+  <si>
+    <t>${DB_Password}</t>
+  </si>
+  <si>
+    <t>${DB_Host}</t>
+  </si>
+  <si>
+    <t>${DB_Port}</t>
+  </si>
+  <si>
+    <t>TestDB</t>
+  </si>
+  <si>
+    <t>sa</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>localhost</t>
+  </si>
+  <si>
+    <t>${DB_User_Name}</t>
   </si>
 </sst>
 </file>
@@ -366,43 +369,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B2" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
+      </c>
+      <c r="E2">
+        <v>1521</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Asif added Graph validation Keywords
</commit_message>
<xml_diff>
--- a/TestData/Database.xlsx
+++ b/TestData/Database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10656162\MyProject\BPxPoc\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JW233CE\BPxPoc\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5FF94EF-9AB2-4C15-8692-FFD662F0160C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23976C40-A5D9-40EA-A9C7-F80BD551F86A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>${DB_Name}</t>
   </si>
@@ -42,16 +42,28 @@
     <t>TestDB</t>
   </si>
   <si>
-    <t>sa</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
     <t>localhost</t>
   </si>
   <si>
     <t>${DB_User_Name}</t>
+  </si>
+  <si>
+    <t>Test User name</t>
+  </si>
+  <si>
+    <t>Test Password</t>
+  </si>
+  <si>
+    <t>TestDB2</t>
+  </si>
+  <si>
+    <t>Test User name2</t>
+  </si>
+  <si>
+    <t>Test Password2</t>
+  </si>
+  <si>
+    <t>localhost2</t>
   </si>
 </sst>
 </file>
@@ -369,10 +381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -389,7 +401,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -406,16 +418,33 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
       </c>
       <c r="E2">
         <v>1521</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3">
+        <v>15212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>